<commit_message>
import tree widget and its dependency;
</commit_message>
<xml_diff>
--- a/app/res/xls/project_property_豆豆项目基本信息模板.xlsx
+++ b/app/res/xls/project_property_豆豆项目基本信息模板.xlsx
@@ -77,7 +77,7 @@
     <t>两厢，三厢，suv，mpv</t>
   </si>
   <si>
-    <t>车型</t>
+    <t>车型 统计的时候的横坐标</t>
   </si>
   <si>
     <t>Engine</t>
@@ -241,7 +241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -253,14 +253,14 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="20"/>
@@ -287,6 +287,11 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b val="1"/>
@@ -327,9 +332,7 @@
       <left style="medium">
         <color indexed="8"/>
       </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="8"/>
       </top>
@@ -339,9 +342,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="8"/>
       </right>
@@ -484,7 +485,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -498,7 +499,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="9" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -510,7 +511,7 @@
     <xf numFmtId="1" fontId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -522,22 +523,22 @@
     <xf numFmtId="1" fontId="6" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="9" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="9" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="9" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -569,15 +570,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>716716</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>151209</xdr:rowOff>
+      <xdr:colOff>731479</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>64294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1011991</xdr:colOff>
+      <xdr:colOff>1026754</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>17859</xdr:rowOff>
+      <xdr:rowOff>92868</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -586,7 +587,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5999638" y="12886134"/>
+          <a:off x="6014679" y="12961143"/>
           <a:ext cx="295276" cy="1000126"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="295275" cy="1000125"/>
@@ -624,7 +625,7 @@
       </xdr:sp>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="3" name="image1.pdf"/>
+          <xdr:cNvPr id="3" name="image2.png"/>
           <xdr:cNvPicPr/>
         </xdr:nvPicPr>
         <xdr:blipFill>
@@ -1892,9 +1893,9 @@
   <sheetFormatPr defaultColWidth="35.75" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.2734" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.0469" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.0391" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35" style="1" customWidth="1"/>
     <col min="5" max="5" width="35.75" style="1" customWidth="1"/>
     <col min="6" max="256" width="35.75" style="1" customWidth="1"/>
   </cols>

</xml_diff>